<commit_message>
Character sheet and skilsl update
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/skills.xlsx
+++ b/CoreRulebook/Data/skills.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="160">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -93,12 +93,6 @@
 \\ 5: Complex weapons </t>
   </si>
   <si>
-    <t xml:space="preserve">Flying Lessons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At Beginner level, you become proficient in using broomsticks, and may use them to fly. Flight related checks gain a + 1 / 2 / 3 / 4 / 5 boost.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Catastrophic Critical</t>
   </si>
   <si>
@@ -176,6 +170,12 @@
     <t xml:space="preserve">Adept Battlemage</t>
   </si>
   <si>
+    <t xml:space="preserve">Flying Lessons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At Beginner level, you become proficient in using broomsticks, and may use them to fly. Flight related checks gain a + 1 / 2 / 3 / 4 / 5 boost.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Focussed Caster</t>
   </si>
   <si>
@@ -222,6 +222,12 @@
     <t xml:space="preserve">Adept Defender</t>
   </si>
   <si>
+    <t xml:space="preserve">Merciful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You may attempt to turn a lethal blow into a knockout strike. When performing an attack that would otherwise kill the target, perform a DV 6 FIN (Precision) check. If it passes, the target is knocked unconscious, rather than killed. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Metamorphmagus</t>
   </si>
   <si>
@@ -235,6 +241,12 @@
   </si>
   <si>
     <t xml:space="preserve">CHR &gt; 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your speed increases by 1m</t>
   </si>
   <si>
     <t xml:space="preserve">Momentum Dodge</t>
@@ -338,7 +350,7 @@
     <t xml:space="preserve">Sleight of Hand</t>
   </si>
   <si>
-    <t xml:space="preserve">If a muggle catches you doing magic, perform a CHR (dexterity) check (difficulty 16) using sleight of hand to convince them that your magic is just trickery.</t>
+    <t xml:space="preserve">If a muggle catches you doing magic, perform a CHR (dexterity) check (DV 16) using sleight of hand to convince them that your magic is just trickery. You may also use this ability in combat to distract an opponent within 2m, causing the next attack on them to take Check Advantage on the damage-causing check. </t>
   </si>
   <si>
     <t xml:space="preserve">FIN &gt; 14</t>
@@ -351,6 +363,15 @@
 You are able to use Charms which match your skill in this skill.</t>
   </si>
   <si>
+    <t xml:space="preserve">Spellbinder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain a +1/2/3/4/5 point bonus on enchanting checks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adept Thaumaturge</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spellmaker</t>
   </si>
   <si>
@@ -361,6 +382,12 @@
     <t xml:space="preserve">Master in at least one school</t>
   </si>
   <si>
+    <t xml:space="preserve">Stabiliser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For each level of this skill, you may nominate one check type (i.e. Illusion spellcasting, lockpicking, persuasion etc.). When performing a check of the nominated type, if possible you may choose to `split the roll’ and instead cast two die of half the nominated value, i.e. 2d10 instead of 1d20. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Surge</t>
   </si>
   <si>
@@ -381,6 +408,18 @@
   <si>
     <t xml:space="preserve">May use a 1d6/8/10/12/20 die to cast Transfiguration spells \\
 You are able to use Transfiguration spells which match your level in this skill.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tool-User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose a new tool to become proficient in. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tough as Nails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you gain this skill, your Max HP increases by an amount equal to twice your level. Thereafter, gain +2 to your max HP every time you level up.</t>
   </si>
   <si>
     <t xml:space="preserve">Undead Benefactor</t>
@@ -490,33 +529,6 @@
   </si>
   <si>
     <t xml:space="preserve">When the full Moon rises, you take the form of a mindless beast (controlled by the GM) for 12 hours, unless the Wolfsbane potion is taken.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spellbinder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain a +1/2/3/4/5 point bonus on enchanting checks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adept Thaumaturge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tool-User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose a new tool to become proficient in. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merciful</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You may attempt to turn a lethal blow into a knockout strike. When performing an attack that would otherwise kill the target, perform a DV 6 FIN (Precision) check. If it passes, the target is knocked unconscious, rather than killed. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stabiliser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For each level of this skill, you may nominate one check type (i.e. Illusion spellcasting, lockpicking, persuasion etc.). When performing a check of the nominated type, if possible you may choose to `split the roll’ and instead cast two die of half the nominated value, i.e. 2d10 instead of 1d20. </t>
   </si>
 </sst>
 </file>
@@ -621,25 +633,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
-      <selection pane="bottomRight" activeCell="D61" activeCellId="0" sqref="D61"/>
+      <selection pane="bottomLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+      <selection pane="bottomRight" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="95.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.12"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -656,7 +668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -673,7 +685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
@@ -690,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
@@ -707,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>14</v>
       </c>
@@ -721,7 +733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -738,7 +750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -755,7 +767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>21</v>
       </c>
@@ -769,55 +781,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D9" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>30</v>
       </c>
@@ -827,42 +839,42 @@
       <c r="C12" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="D12" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="E13" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>36</v>
       </c>
@@ -876,55 +888,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="D17" s="0" t="s">
+        <v>43</v>
+      </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>46</v>
       </c>
@@ -938,7 +950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>48</v>
       </c>
@@ -955,7 +967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>51</v>
       </c>
@@ -972,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>54</v>
       </c>
@@ -986,7 +998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>56</v>
       </c>
@@ -1003,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>58</v>
       </c>
@@ -1020,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>61</v>
       </c>
@@ -1030,14 +1042,11 @@
       <c r="C25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E25" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>63</v>
       </c>
@@ -1047,577 +1056,632 @@
       <c r="C26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="E27" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="E28" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="B29" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="E29" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="E30" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="B31" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="0" t="s">
         <v>77</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>78</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>79</v>
       </c>
       <c r="D32" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="B33" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="E33" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="B34" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E33" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="D34" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="E34" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="E36" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="E36" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="E37" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E37" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38" s="0" t="n">
+      <c r="C39" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="E39" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="C40" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="E40" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="B41" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="E42" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="E42" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="B43" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B43" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="E43" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="E43" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="B44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B44" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="E44" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>112</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="E45" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="E45" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="B46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="E46" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="B47" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E46" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="D47" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B47" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="E47" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="E47" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="B48" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="B49" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E48" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="E49" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="B49" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="B50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E49" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="E50" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B50" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="B51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D51" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="E50" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="E51" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="B51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="B52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D52" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="E51" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="E52" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="B52" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="B53" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="E53" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="E52" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="B54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="D54" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="E54" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="E53" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="B55" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B54" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="E55" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="D54" s="0" t="s">
+      <c r="B56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E54" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="D56" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B55" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="E56" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="D55" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="E55" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="B57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B56" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="D57" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="E57" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="E56" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="B58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B57" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="D58" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="D57" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="E57" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="E58" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B58" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="B59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D59" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="E58" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="E59" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="B59" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="B60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E59" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="D60" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B60" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="E60" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="E60" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="B61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B61" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="E61" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="B62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="0"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C65" s="0"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="0"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="0"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="0"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="0"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="0"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Spellcasting overhaul nearly completed
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/skills.xlsx
+++ b/CoreRulebook/Data/skills.xlsx
@@ -11,9 +11,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$52</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$40</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$D$39</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$40</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$52</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">Merciful</t>
   </si>
   <si>
-    <t xml:space="preserve">You may attempt to turn a lethal blow into a knockout strike. When performing an attack that would otherwise kill the target, perform a DV 8 \attFIN{} check. If it passes, the target is knocked unconscious, rather than killed. </t>
+    <t xml:space="preserve">You may attempt to turn a lethal blow into a knockout strike. When performing an attack that would otherwise kill the target, perform a DV 8 \attFin{} check. If it passes, the target is knocked unconscious, rather than killed. </t>
   </si>
   <si>
     <t xml:space="preserve">Mimicry</t>
@@ -370,7 +370,7 @@
     <t xml:space="preserve">Weapons: Long Range Threat</t>
   </si>
   <si>
-    <t xml:space="preserve">You are considered proficient in the use of more complex ranged weapons: bows &amp; crossbows</t>
+    <t xml:space="preserve">You are considered proficient in the use of more complex ranged weapons: bows \&amp; crossbows</t>
   </si>
   <si>
     <t xml:space="preserve">Weapons: Simple Ranged Training</t>
@@ -504,17 +504,17 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="95.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.57"/>
   </cols>
   <sheetData>
@@ -1164,7 +1164,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:D52"/>
+  <autoFilter ref="A1:D40"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Runecaster moved out of skills
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/skills.xlsx
+++ b/CoreRulebook/Data/skills.xlsx
@@ -11,9 +11,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$47</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$D$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$35</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$46</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$D$33</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$34</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -239,18 +239,6 @@
   </si>
   <si>
     <t xml:space="preserve">Spells that normally require an incantation can be used silently. You may only silently cast spells which you have already memorised, but you must perform a casting check for all spells cast silently.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Runecaster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Once per day, you may utilise your knowledge of the ancient {\it Enchanting Runes} to form a magic spell from the endless chaos of primordial magic. 
-As with the usual enchanting process, you must trace the runes out in the air over the course of a major action, describing what effect you would like this runechain to have. The GM then decides the spellschool and the difficulty of the described spell, based on the magnitude of the effect you are trying to create. You must then perform a casting check to realise the runecast. 
-Runecasting is almost always weaker than a spell cast using the normal methods, though it provides much greater flexibility. You cannot runecast to exactly replicate the effects of an existing spell. 
-After successfully performing a Runecast, you may spend 6 hours translating the runechain into a conventional incantation-based spell, with the discipline and DV set by the GM. You may then memory-cast this spell, and others may book-cast it, as they would any other spell.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adept Spellcaster</t>
   </si>
   <si>
     <t xml:space="preserve">Sprint Start</t>
@@ -489,9 +477,9 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -859,235 +847,222 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="48.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>69</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="48.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="0" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C33" s="1" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" s="1" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="B42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="B43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" s="1" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="83.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="B48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1" t="s">
+    </row>
+    <row r="49" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="83.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="B49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B49" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="36.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="B50" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1119,7 +1094,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:D47"/>
+  <autoFilter ref="A1:D46"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>